<commit_message>
add ups in inventory
</commit_message>
<xml_diff>
--- a/wwwroot/RegulatorExcel/InputTemplate/Inventory.xlsx
+++ b/wwwroot/RegulatorExcel/InputTemplate/Inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29704"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Git\SLA_Management\wwwroot\GatewayExcel\InputTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{698110EF-25A5-4247-9223-F4B617E1EE78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C113889-F3BB-4590-92AD-9CF2862DC662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="345" windowWidth="19875" windowHeight="7725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$I$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$5:$J$5</definedName>
   </definedNames>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Inventory Maintenance</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Terminal Name</t>
+  </si>
+  <si>
+    <t>UPS</t>
   </si>
   <si>
     <t>Connected</t>
@@ -591,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:S5"/>
+  <dimension ref="A2:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView tabSelected="1" topLeftCell="D2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -603,25 +606,25 @@
     <col min="2" max="2" width="22.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.75" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32.375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="36.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="50.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="10.875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="12.875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16" style="1" customWidth="1"/>
-    <col min="15" max="15" width="26" style="1" customWidth="1"/>
-    <col min="16" max="16" width="23.375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14" style="1" customWidth="1"/>
-    <col min="18" max="18" width="32" style="1" customWidth="1"/>
-    <col min="19" max="19" width="32.25" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="1"/>
+    <col min="5" max="6" width="31.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.75" style="1" customWidth="1"/>
+    <col min="9" max="9" width="32.375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="50.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13.375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16" style="1" customWidth="1"/>
+    <col min="16" max="16" width="26" style="1" customWidth="1"/>
+    <col min="17" max="17" width="23.375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14" style="1" customWidth="1"/>
+    <col min="19" max="19" width="32" style="1" customWidth="1"/>
+    <col min="20" max="20" width="32.25" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" ht="18" customHeight="1">
+    <row r="2" spans="1:20" ht="18" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -642,9 +645,10 @@
       <c r="P2" s="7"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="7"/>
-      <c r="S2" s="8"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="8"/>
     </row>
-    <row r="3" spans="1:19" ht="18" customHeight="1">
+    <row r="3" spans="1:20" ht="18" customHeight="1">
       <c r="A3" s="9"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -663,14 +667,15 @@
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
-      <c r="S3" s="11"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
     </row>
-    <row r="4" spans="1:19" ht="15">
+    <row r="4" spans="1:20" ht="15">
       <c r="A4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:19" ht="16.5" customHeight="1">
+    <row r="5" spans="1:20" ht="16.5" customHeight="1">
       <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
@@ -686,7 +691,7 @@
       <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -727,11 +732,14 @@
       </c>
       <c r="S5" s="5" t="s">
         <v>19</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:S3"/>
+    <mergeCell ref="A2:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="63" orientation="portrait"/>

</xml_diff>